<commit_message>
Selected some BOM components.
</commit_message>
<xml_diff>
--- a/KiCad/Power_Board/BOM.xlsx
+++ b/KiCad/Power_Board/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="142">
   <si>
     <t>REFDES</t>
   </si>
@@ -111,9 +111,6 @@
     <t>0.1uF Cap</t>
   </si>
   <si>
-    <t>1uF Cap</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>3.3uH Inductor</t>
   </si>
   <si>
-    <t>10uF Cap</t>
-  </si>
-  <si>
     <t>0ohm Jumper</t>
   </si>
   <si>
@@ -180,9 +174,6 @@
     <t>520k Resistor</t>
   </si>
   <si>
-    <t>L1,L2,L3, L5</t>
-  </si>
-  <si>
     <t>U4,U5,U6,U9</t>
   </si>
   <si>
@@ -219,18 +210,12 @@
     <t>U8</t>
   </si>
   <si>
-    <t>L7</t>
-  </si>
-  <si>
     <t>U10</t>
   </si>
   <si>
     <t>U11</t>
   </si>
   <si>
-    <t>MAX152x</t>
-  </si>
-  <si>
     <t>U7</t>
   </si>
   <si>
@@ -400,6 +385,63 @@
   </si>
   <si>
     <t>R9,R10,R11,R22,R23,R30,R31,R32</t>
+  </si>
+  <si>
+    <t>10uF Cap (25V X7R 10%)</t>
+  </si>
+  <si>
+    <t>490-5307-1-ND</t>
+  </si>
+  <si>
+    <t>GRM188R71E105KA12D</t>
+  </si>
+  <si>
+    <t>1uF Cap (25V X7R 10%)</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>1210</t>
+  </si>
+  <si>
+    <t>490-6544-1-ND</t>
+  </si>
+  <si>
+    <t>GRM32ER71H106KA12L</t>
+  </si>
+  <si>
+    <t>L1,L2,L3, L5,L7</t>
+  </si>
+  <si>
+    <t>587-3459-1-ND</t>
+  </si>
+  <si>
+    <t>NRS5030T3R3MMGJ</t>
+  </si>
+  <si>
+    <t>587-3462-1-ND</t>
+  </si>
+  <si>
+    <t>NRS5030T6R8MMGJ</t>
+  </si>
+  <si>
+    <t>587-2731-1-ND</t>
+  </si>
+  <si>
+    <t>NS12555T470MN</t>
+  </si>
+  <si>
+    <t>MAX1523EUT+TCT-ND</t>
+  </si>
+  <si>
+    <t>MAX1523</t>
+  </si>
+  <si>
+    <t>DFLS240LDICT-ND</t>
   </si>
 </sst>
 </file>
@@ -409,7 +451,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,6 +473,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -440,7 +488,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -457,12 +505,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -475,32 +532,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -808,10 +854,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,58 +866,63 @@
     <col min="1" max="1" width="59.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="16" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="C1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2">
-        <f t="shared" ref="B2:B50" si="0">1+LEN(A2)-LEN(SUBSTITUTE(A2,",",""))</f>
+        <f t="shared" ref="B2:B49" si="0">1+LEN(A2)-LEN(SUBSTITUTE(A2,",",""))</f>
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -881,35 +933,36 @@
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2">
-        <f t="shared" ref="G2:G50" si="1">B2</f>
+      <c r="G2" s="14"/>
+      <c r="H2" s="2">
+        <f>B2</f>
         <v>4</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>10</v>
       </c>
-      <c r="I2" s="2">
-        <f t="shared" ref="I2:I50" si="2">H2-G2</f>
+      <c r="J2" s="2">
+        <f t="shared" ref="J2:J49" si="1">I2-H2</f>
         <v>6</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>2.25</v>
       </c>
-      <c r="K2" s="1">
-        <f t="shared" ref="K2:K9" si="3">H2*J2</f>
+      <c r="L2" s="1">
+        <f t="shared" ref="L2:L49" si="2">I2*K2</f>
         <v>22.5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B3" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
@@ -920,38 +973,39 @@
       <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+      <c r="G3" s="14"/>
       <c r="H3" s="2">
+        <f>B3</f>
         <v>1</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
         <v>5.99</v>
       </c>
-      <c r="K3" s="1">
-        <f t="shared" si="3"/>
-        <v>5.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="1">
+        <f t="shared" si="2"/>
+        <v>17.97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
@@ -959,38 +1013,39 @@
       <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+      <c r="G4" s="14"/>
       <c r="H4" s="2">
+        <f>B4</f>
         <v>1</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K4" s="1">
         <v>3.06</v>
       </c>
-      <c r="K4" s="1">
-        <f t="shared" si="3"/>
-        <v>3.06</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="1">
+        <f t="shared" si="2"/>
+        <v>9.18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>13</v>
@@ -998,35 +1053,36 @@
       <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+      <c r="G5" s="14"/>
       <c r="H5" s="2">
+        <f>B5</f>
         <v>1</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
+        <v>3</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K5" s="1">
         <v>3.65</v>
       </c>
-      <c r="K5" s="1">
-        <f t="shared" si="3"/>
-        <v>3.65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="1">
+        <f t="shared" si="2"/>
+        <v>10.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -1037,72 +1093,76 @@
       <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+      <c r="G6" s="14"/>
       <c r="H6" s="2">
+        <f>B6</f>
         <v>1</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K6" s="1">
         <v>2.76</v>
       </c>
-      <c r="K6" s="1">
-        <f t="shared" si="3"/>
-        <v>2.76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="1">
+        <f t="shared" si="2"/>
+        <v>8.2799999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="E7" s="5" t="s">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+      <c r="G7" s="14"/>
       <c r="H7" s="2">
+        <f>B7</f>
         <v>1</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="1">
-        <v>4.8</v>
+        <v>3</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="3"/>
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3.84</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="2"/>
+        <v>11.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>19</v>
@@ -1113,35 +1173,36 @@
       <c r="F8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="2">
-        <f t="shared" si="1"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="2">
+        <f>B8</f>
         <v>2</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>2</v>
       </c>
-      <c r="I8" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
+      <c r="J8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
         <v>12.97</v>
       </c>
-      <c r="K8" s="1">
-        <f t="shared" si="3"/>
+      <c r="L8" s="1">
+        <f t="shared" si="2"/>
         <v>25.94</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -1152,28 +1213,29 @@
       <c r="F9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+      <c r="G9" s="14"/>
       <c r="H9" s="2">
+        <f>B9</f>
         <v>1</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
         <v>2.27</v>
       </c>
-      <c r="K9" s="1">
-        <f t="shared" si="3"/>
+      <c r="L9" s="1">
+        <f t="shared" si="2"/>
         <v>2.27</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" si="0"/>
@@ -1181,53 +1243,69 @@
       </c>
       <c r="C10" s="2"/>
       <c r="E10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2">
-        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="2">
+        <f>B10</f>
+        <v>1</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>141</v>
+      </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="2">
+        <f>B11</f>
         <v>2</v>
       </c>
-      <c r="H11" s="2"/>
       <c r="I11" s="2">
-        <f t="shared" si="2"/>
-        <v>-2</v>
-      </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="2"/>
+        <v>2.3000000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" si="0"/>
@@ -1235,26 +1313,29 @@
       </c>
       <c r="C12" s="2"/>
       <c r="E12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2">
-        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="2">
+        <f>B12</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" si="0"/>
@@ -1262,146 +1343,203 @@
       </c>
       <c r="C13" s="2"/>
       <c r="E13" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2">
-        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="2">
+        <f>B13</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>132</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" t="s">
+        <v>134</v>
+      </c>
       <c r="F14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H14" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="2">
+        <f>B14</f>
+        <v>5</v>
+      </c>
       <c r="I14" s="2">
-        <f t="shared" si="2"/>
-        <v>-4</v>
-      </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="2"/>
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" t="s">
+        <v>136</v>
+      </c>
       <c r="F15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H15" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="2">
+        <f>B15</f>
+        <v>1</v>
+      </c>
       <c r="I15" s="2">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="2"/>
+        <v>1.3800000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" t="s">
+        <v>138</v>
+      </c>
       <c r="F16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H16" s="2"/>
+        <v>105</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="2">
+        <f>B16</f>
+        <v>1</v>
+      </c>
       <c r="I16" s="2">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1.41</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="2"/>
+        <v>4.2299999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G17" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="2">
+        <f>B17</f>
+        <v>8</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2">
+        <f t="shared" si="1"/>
+        <v>-8</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2">
-        <f t="shared" si="2"/>
-        <v>-8</v>
-      </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="2">
+        <f>B18</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" si="0"/>
@@ -1409,23 +1547,26 @@
       </c>
       <c r="C19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G19" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2">
-        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="2">
+        <f>B19</f>
+        <v>1</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" si="0"/>
@@ -1433,68 +1574,78 @@
       </c>
       <c r="C20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2">
-        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="2">
+        <f>B20</f>
+        <v>1</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G21" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="2">
+        <f>B21</f>
+        <v>3</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="B22" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I22" s="2">
-        <f t="shared" si="2"/>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="2">
+        <f>B22</f>
+        <v>1</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="B23" s="2">
         <f t="shared" si="0"/>
@@ -1502,20 +1653,25 @@
       </c>
       <c r="C23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I23" s="2">
-        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="2">
+        <f>B23</f>
+        <v>1</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" si="0"/>
@@ -1523,20 +1679,25 @@
       </c>
       <c r="C24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G24" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I24" s="2">
-        <f t="shared" si="2"/>
+        <v>115</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="2">
+        <f>B24</f>
+        <v>1</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="0"/>
@@ -1544,20 +1705,25 @@
       </c>
       <c r="C25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I25" s="2">
-        <f t="shared" si="2"/>
+        <v>97</v>
+      </c>
+      <c r="G25" s="14"/>
+      <c r="H25" s="2">
+        <f>B25</f>
+        <v>1</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="0"/>
@@ -1565,20 +1731,25 @@
       </c>
       <c r="C26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G26" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I26" s="2">
-        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="2">
+        <f>B26</f>
+        <v>1</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="B27" s="2">
         <f t="shared" si="0"/>
@@ -1586,20 +1757,25 @@
       </c>
       <c r="C27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G27" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I27" s="2">
-        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="G27" s="14"/>
+      <c r="H27" s="2">
+        <f>B27</f>
+        <v>1</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" si="0"/>
@@ -1607,20 +1783,25 @@
       </c>
       <c r="C28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G28" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I28" s="2">
-        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="2">
+        <f>B28</f>
+        <v>1</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="B29" s="2">
         <f t="shared" si="0"/>
@@ -1628,62 +1809,77 @@
       </c>
       <c r="C29" s="2"/>
       <c r="F29" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G29" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I29" s="2">
-        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="G29" s="14"/>
+      <c r="H29" s="2">
+        <f>B29</f>
+        <v>1</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" s="2"/>
       <c r="F30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G30" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I30" s="2">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="G30" s="14"/>
+      <c r="H30" s="2">
+        <f>B30</f>
+        <v>2</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B31" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" s="2"/>
       <c r="F31" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G31" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I31" s="2">
-        <f t="shared" si="2"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="G31" s="14"/>
+      <c r="H31" s="2">
+        <f>B31</f>
+        <v>1</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="B32" s="2">
         <f t="shared" si="0"/>
@@ -1691,20 +1887,25 @@
       </c>
       <c r="C32" s="2"/>
       <c r="F32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G32" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I32" s="2">
-        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+      <c r="G32" s="14"/>
+      <c r="H32" s="2">
+        <f>B32</f>
+        <v>1</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L32" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>50</v>
       </c>
       <c r="B33" s="2">
         <f t="shared" si="0"/>
@@ -1712,20 +1913,25 @@
       </c>
       <c r="C33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G33" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I33" s="2">
-        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="G33" s="14"/>
+      <c r="H33" s="2">
+        <f>B33</f>
+        <v>1</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L33" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B34" s="2">
         <f t="shared" si="0"/>
@@ -1733,62 +1939,77 @@
       </c>
       <c r="C34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G34" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I34" s="2">
-        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="H34" s="2">
+        <f>B34</f>
+        <v>1</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L34" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B35" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G35" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I35" s="2">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="G35" s="14"/>
+      <c r="H35" s="2">
+        <f>B35</f>
+        <v>2</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="L35" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B36" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G36" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I36" s="2">
-        <f t="shared" si="2"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="G36" s="14"/>
+      <c r="H36" s="2">
+        <f>B36</f>
+        <v>1</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="L36" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B37" s="2">
         <f t="shared" si="0"/>
@@ -1796,20 +2017,25 @@
       </c>
       <c r="C37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G37" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I37" s="2">
-        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="G37" s="14"/>
+      <c r="H37" s="2">
+        <f>B37</f>
+        <v>1</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L37" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="B38" s="2">
         <f t="shared" si="0"/>
@@ -1817,41 +2043,51 @@
       </c>
       <c r="C38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G38" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I38" s="2">
-        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+      <c r="G38" s="14"/>
+      <c r="H38" s="2">
+        <f>B38</f>
+        <v>1</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L38" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="B39" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G39" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I39" s="2">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="G39" s="14"/>
+      <c r="H39" s="2">
+        <f>B39</f>
+        <v>2</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="L39" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B40" s="2">
         <f t="shared" si="0"/>
@@ -1859,238 +2095,295 @@
       </c>
       <c r="C40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G40" s="2">
-        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="G40" s="14"/>
+      <c r="H40" s="2">
+        <f>B40</f>
         <v>2</v>
       </c>
-      <c r="I40" s="2">
-        <f t="shared" si="2"/>
+      <c r="J40" s="2">
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L40" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="B41" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G41" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I41" s="2">
-        <f t="shared" si="2"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G41" s="14"/>
+      <c r="H41" s="2">
+        <f>B41</f>
+        <v>7</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="1"/>
+        <v>-7</v>
+      </c>
+      <c r="L41" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="B42" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C42" s="2"/>
+      <c r="C42" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" t="s">
+        <v>124</v>
+      </c>
+      <c r="E42" t="s">
+        <v>125</v>
+      </c>
       <c r="F42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G42" s="2">
-        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H42" s="2">
+        <f>B42</f>
         <v>7</v>
       </c>
-      <c r="I42" s="2">
-        <f t="shared" si="2"/>
+      <c r="J42" s="2">
+        <f t="shared" si="1"/>
         <v>-7</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L42" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="B43" s="2">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C43" s="2"/>
       <c r="F43" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G43" s="2">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="I43" s="2">
-        <f t="shared" si="2"/>
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="G43" s="14"/>
+      <c r="H43" s="2">
+        <f>B43</f>
+        <v>1</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="L43" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="B44" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G44" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I44" s="2">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="G44" s="14"/>
+      <c r="H44" s="2">
+        <f>B44</f>
+        <v>3</v>
+      </c>
+      <c r="J44" s="2">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="L44" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="B45" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>1+LEN(A45)-LEN(SUBSTITUTE(A45,",",""))</f>
+        <v>1</v>
       </c>
       <c r="C45" s="2"/>
       <c r="F45" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G45" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I45" s="2">
-        <f t="shared" si="2"/>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G45" s="14"/>
+      <c r="H45" s="2">
+        <f>B45</f>
+        <v>1</v>
+      </c>
+      <c r="J45" s="2">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="L45" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="B46" s="2">
         <f>1+LEN(A46)-LEN(SUBSTITUTE(A46,",",""))</f>
-        <v>1</v>
-      </c>
-      <c r="C46" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E46" t="s">
+        <v>131</v>
+      </c>
       <c r="F46" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G46" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I46" s="2">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="H46" s="2">
+        <f>B46</f>
+        <v>16</v>
+      </c>
+      <c r="I46">
+        <v>50</v>
+      </c>
+      <c r="J46" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="K46" s="1">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="L46" s="1">
+        <f t="shared" si="2"/>
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B47" s="2">
         <f>1+LEN(A47)-LEN(SUBSTITUTE(A47,",",""))</f>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G47" s="2">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="I47" s="2">
-        <f t="shared" si="2"/>
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="G47" s="14"/>
+      <c r="H47" s="2">
+        <f>B47</f>
+        <v>1</v>
+      </c>
+      <c r="J47" s="2">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="L47" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="B48" s="2">
-        <f>1+LEN(A48)-LEN(SUBSTITUTE(A48,",",""))</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="C48" s="2"/>
       <c r="F48" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G48" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I48" s="2">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="G48" s="14"/>
+      <c r="H48" s="2">
+        <f>B48</f>
+        <v>8</v>
+      </c>
+      <c r="J48" s="2">
+        <f t="shared" si="1"/>
+        <v>-8</v>
+      </c>
+      <c r="L48" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B49" s="2">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C49" s="2"/>
       <c r="F49" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G49" s="2">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="I49" s="2">
-        <f t="shared" si="2"/>
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50" s="2">
-        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="G49" s="14"/>
+      <c r="H49" s="2">
+        <f>B49</f>
         <v>6</v>
       </c>
-      <c r="C50" s="2"/>
-      <c r="F50" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G50" s="2">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="I50" s="2">
-        <f t="shared" si="2"/>
+      <c r="J49" s="2">
+        <f t="shared" si="1"/>
         <v>-6</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="L49" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K51" s="7">
-        <f>SUM(K2:K50)</f>
-        <v>70.97</v>
+      <c r="G50" s="15"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="7">
+        <f>SUM(L2:L49)</f>
+        <v>141.41999999999999</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:I1048576">
+  <conditionalFormatting sqref="J1:J1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated BOM & Schematic
BOM was too high.

Switched to a cheaper 8bit DAC. This will still yield ~0.06V resolution
when gained up to +15V.

Currently leaving power circuits alone, but in the future this could be
better optimized for space and cost. Multichannel buck PMIC would be a
good option to simplify the digital supplies.
</commit_message>
<xml_diff>
--- a/KiCad/Power_Board/BOM.xlsx
+++ b/KiCad/Power_Board/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="207">
   <si>
     <t>REFDES</t>
   </si>
@@ -75,15 +75,6 @@
     <t>50V Boost</t>
   </si>
   <si>
-    <t>296-27741-1-ND</t>
-  </si>
-  <si>
-    <t>DAC7578</t>
-  </si>
-  <si>
-    <t>8 Channel DAC</t>
-  </si>
-  <si>
     <t>AD1583BRTZ-REEL7CT-ND</t>
   </si>
   <si>
@@ -628,6 +619,24 @@
   </si>
   <si>
     <t>CUT TO SIZE</t>
+  </si>
+  <si>
+    <t>Board Total</t>
+  </si>
+  <si>
+    <t>Order Total</t>
+  </si>
+  <si>
+    <t>Boards Possible</t>
+  </si>
+  <si>
+    <t>MAX5259</t>
+  </si>
+  <si>
+    <t>MAX5259EEE+-ND</t>
+  </si>
+  <si>
+    <t>8 Channel 8bit DAC</t>
   </si>
 </sst>
 </file>
@@ -1044,11 +1053,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,23 +1070,25 @@
     <col min="7" max="7" width="15.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="10" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
@@ -1085,34 +1096,40 @@
         <v>2</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2">
         <f t="shared" ref="B2:B47" si="0">1+LEN(A2)-LEN(SUBSTITUTE(A2,",",""))</f>
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -1135,24 +1152,32 @@
         <f t="shared" ref="J2:J47" si="2">I2-H2</f>
         <v>6</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="2">
+        <f>FLOOR(I2/H2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="L2" s="1">
         <v>2.25</v>
       </c>
-      <c r="L2" s="1">
-        <f t="shared" ref="L2:L47" si="3">I2*K2</f>
+      <c r="M2" s="1">
+        <f>H2*L2</f>
+        <v>9</v>
+      </c>
+      <c r="N2" s="1">
+        <f>I2*L2</f>
         <v>22.5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
@@ -1169,33 +1194,41 @@
         <v>1</v>
       </c>
       <c r="I3" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K47" si="3">FLOOR(I3/H3,1)</f>
+        <v>2</v>
+      </c>
+      <c r="L3" s="1">
         <v>5.99</v>
       </c>
-      <c r="L3" s="1">
-        <f t="shared" si="3"/>
-        <v>17.97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="1">
+        <f>H3*L3</f>
+        <v>5.99</v>
+      </c>
+      <c r="N3" s="1">
+        <f>I3*L3</f>
+        <v>11.98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
@@ -1209,33 +1242,41 @@
         <v>1</v>
       </c>
       <c r="I4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L4" s="1">
         <v>3.06</v>
       </c>
-      <c r="L4" s="1">
-        <f t="shared" si="3"/>
-        <v>9.18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="1">
+        <f>H4*L4</f>
+        <v>3.06</v>
+      </c>
+      <c r="N4" s="1">
+        <f>I4*L4</f>
+        <v>6.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>13</v>
@@ -1249,30 +1290,38 @@
         <v>1</v>
       </c>
       <c r="I5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L5" s="1">
         <v>3.65</v>
       </c>
-      <c r="L5" s="1">
-        <f t="shared" si="3"/>
-        <v>10.95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="1">
+        <f>H5*L5</f>
+        <v>3.65</v>
+      </c>
+      <c r="N5" s="1">
+        <f>I5*L5</f>
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -1289,36 +1338,44 @@
         <v>1</v>
       </c>
       <c r="I6" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L6" s="1">
         <v>2.76</v>
       </c>
-      <c r="L6" s="1">
-        <f t="shared" si="3"/>
-        <v>8.2799999999999994</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="1">
+        <f>H6*L6</f>
+        <v>2.76</v>
+      </c>
+      <c r="N6" s="1">
+        <f>I6*L6</f>
+        <v>5.52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>18</v>
@@ -1329,39 +1386,47 @@
         <v>1</v>
       </c>
       <c r="I7" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L7" s="1">
         <v>3.84</v>
       </c>
-      <c r="L7" s="1">
-        <f t="shared" si="3"/>
-        <v>11.52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="1">
+        <f>H7*L7</f>
+        <v>3.84</v>
+      </c>
+      <c r="N7" s="1">
+        <f>I7*L7</f>
+        <v>7.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>205</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>20</v>
+        <v>204</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>21</v>
+        <v>206</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="2">
@@ -1375,33 +1440,41 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="K8" s="1">
-        <v>12.97</v>
+      <c r="K8" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="3"/>
-        <v>51.88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.82</v>
+      </c>
+      <c r="M8" s="1">
+        <f>H8*L8</f>
+        <v>5.64</v>
+      </c>
+      <c r="N8" s="1">
+        <f>I8*L8</f>
+        <v>11.28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="2">
@@ -1409,39 +1482,47 @@
         <v>1</v>
       </c>
       <c r="I9" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L9" s="1">
         <v>2.27</v>
       </c>
-      <c r="L9" s="1">
-        <f t="shared" si="3"/>
-        <v>6.8100000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="1">
+        <f>H9*L9</f>
+        <v>2.27</v>
+      </c>
+      <c r="N9" s="1">
+        <f>I9*L9</f>
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="2">
@@ -1449,39 +1530,47 @@
         <v>1</v>
       </c>
       <c r="I10" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="K10" s="1">
+        <v>2</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="L10" s="1">
         <v>0.93</v>
       </c>
-      <c r="L10" s="1">
-        <f t="shared" si="3"/>
-        <v>4.6500000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="1">
+        <f>H10*L10</f>
+        <v>0.93</v>
+      </c>
+      <c r="N10" s="1">
+        <f>I10*L10</f>
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="2">
@@ -1495,33 +1584,41 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L11" s="1">
         <v>0.46</v>
       </c>
-      <c r="L11" s="1">
-        <f t="shared" si="3"/>
+      <c r="M11" s="1">
+        <f>H11*L11</f>
+        <v>0.92</v>
+      </c>
+      <c r="N11" s="1">
+        <f>I11*L11</f>
         <v>2.3000000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="2">
@@ -1535,36 +1632,44 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L12" s="1">
         <v>0.14599999999999999</v>
       </c>
-      <c r="L12" s="1">
-        <f t="shared" si="3"/>
+      <c r="M12" s="1">
+        <f>H12*L12</f>
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="N12" s="1">
+        <f>I12*L12</f>
         <v>1.46</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="G13" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="1"/>
@@ -1577,33 +1682,41 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L13" s="1">
         <v>0.11700000000000001</v>
       </c>
-      <c r="L13" s="1">
-        <f t="shared" si="3"/>
+      <c r="M13" s="1">
+        <f>H13*L13</f>
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="N13" s="1">
+        <f>I13*L13</f>
         <v>1.1700000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="2">
@@ -1617,33 +1730,41 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L14" s="1">
         <v>0.41</v>
       </c>
-      <c r="L14" s="1">
-        <f t="shared" si="3"/>
+      <c r="M14" s="1">
+        <f>H14*L14</f>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="N14" s="1">
+        <f>I14*L14</f>
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="2">
@@ -1657,33 +1778,41 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="L15" s="1">
         <v>0.46</v>
       </c>
-      <c r="L15" s="1">
-        <f t="shared" si="3"/>
+      <c r="M15" s="1">
+        <f>H15*L15</f>
+        <v>0.46</v>
+      </c>
+      <c r="N15" s="1">
+        <f>I15*L15</f>
         <v>1.3800000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="2">
@@ -1691,42 +1820,50 @@
         <v>1</v>
       </c>
       <c r="I16" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L16" s="1">
         <v>1.41</v>
       </c>
-      <c r="L16" s="1">
-        <f t="shared" si="3"/>
-        <v>4.2299999999999995</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="1">
+        <f>H16*L16</f>
+        <v>1.41</v>
+      </c>
+      <c r="N16" s="1">
+        <f>I16*L16</f>
+        <v>2.82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="1"/>
@@ -1739,456 +1876,544 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="L17" s="1">
         <v>0.04</v>
       </c>
-      <c r="L17" s="1">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="1">
+        <f>H17*L17</f>
+        <v>0.32</v>
+      </c>
+      <c r="N17" s="1">
+        <f>I17*L17</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I18" s="2">
+        <v>10</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L18" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M18" s="1">
+        <f>H18*L18</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N18" s="1">
+        <f>I18*L18</f>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I19" s="2">
+        <v>10</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L19" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M19" s="1">
+        <f>H19*L19</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N19" s="1">
+        <f>I19*L19</f>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H18" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I18" s="2">
-        <v>10</v>
-      </c>
-      <c r="J18" s="2">
+      <c r="F20" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I20" s="2">
+        <v>10</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="L20" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M20" s="1">
+        <f>H20*L20</f>
+        <v>0.249</v>
+      </c>
+      <c r="N20" s="1">
+        <f>I20*L20</f>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>10</v>
+      </c>
+      <c r="J21" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="K18" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L18" s="1">
-        <f t="shared" si="3"/>
+      <c r="K21" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L21" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M21" s="1">
+        <f>H21*L21</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N21" s="1">
+        <f>I21*L21</f>
         <v>0.83000000000000007</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H19" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I19" s="2">
-        <v>10</v>
-      </c>
-      <c r="J19" s="2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I22" s="2">
+        <v>10</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="L22" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M22" s="1">
+        <f>H22*L22</f>
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="N22" s="1">
+        <f>I22*L22</f>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I23" s="2">
+        <v>10</v>
+      </c>
+      <c r="J23" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="K19" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L19" s="1">
-        <f t="shared" si="3"/>
+      <c r="K23" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L23" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M23" s="1">
+        <f>H23*L23</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N23" s="1">
+        <f>I23*L23</f>
         <v>0.83000000000000007</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H20" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I20" s="2">
-        <v>10</v>
-      </c>
-      <c r="J20" s="2">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="K20" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L20" s="1">
-        <f t="shared" si="3"/>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I24" s="2">
+        <v>10</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L24" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M24" s="1">
+        <f>H24*L24</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N24" s="1">
+        <f>I24*L24</f>
         <v>0.83000000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H21" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I21" s="2">
-        <v>10</v>
-      </c>
-      <c r="J21" s="2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I25" s="2">
+        <v>10</v>
+      </c>
+      <c r="J25" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="K21" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L21" s="1">
-        <f t="shared" si="3"/>
+      <c r="K25" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L25" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M25" s="1">
+        <f>H25*L25</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N25" s="1">
+        <f>I25*L25</f>
         <v>0.83000000000000007</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B22" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="2" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <v>10</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L26" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M26" s="1">
+        <f>H26*L26</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N26" s="1">
+        <f>I26*L26</f>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H22" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I22" s="2">
-        <v>10</v>
-      </c>
-      <c r="J22" s="2">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="K22" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L22" s="1">
-        <f t="shared" si="3"/>
+      <c r="F27" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I27" s="2">
+        <v>10</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L27" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M27" s="1">
+        <f>H27*L27</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N27" s="1">
+        <f>I27*L27</f>
         <v>0.83000000000000007</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H23" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I23" s="2">
-        <v>10</v>
-      </c>
-      <c r="J23" s="2">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="K23" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L23" s="1">
-        <f t="shared" si="3"/>
-        <v>0.83000000000000007</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H24" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I24" s="2">
-        <v>10</v>
-      </c>
-      <c r="J24" s="2">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="K24" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L24" s="1">
-        <f t="shared" si="3"/>
-        <v>0.83000000000000007</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H25" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I25" s="2">
-        <v>10</v>
-      </c>
-      <c r="J25" s="2">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="K25" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L25" s="1">
-        <f t="shared" si="3"/>
-        <v>0.83000000000000007</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H26" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I26" s="2">
-        <v>10</v>
-      </c>
-      <c r="J26" s="2">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="K26" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L26" s="1">
-        <f t="shared" si="3"/>
-        <v>0.83000000000000007</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H27" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I27" s="2">
-        <v>10</v>
-      </c>
-      <c r="J27" s="2">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="K27" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L27" s="1">
-        <f t="shared" si="3"/>
-        <v>0.83000000000000007</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B28" s="2">
         <f>1+LEN(A28)-LEN(SUBSTITUTE(A28,",",""))</f>
         <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H28" s="2">
         <f>B28</f>
@@ -2201,36 +2426,44 @@
         <f>I28-H28</f>
         <v>8</v>
       </c>
-      <c r="K28" s="1">
-        <v>8.3000000000000004E-2</v>
+      <c r="K28" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="L28" s="1">
-        <f>I28*K28</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M28" s="1">
+        <f>H28*L28</f>
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="N28" s="1">
+        <f>I28*L28</f>
         <v>0.83000000000000007</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B29" s="2">
         <f>1+LEN(A29)-LEN(SUBSTITUTE(A29,",",""))</f>
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H29" s="2">
         <f>B29</f>
@@ -2243,456 +2476,544 @@
         <f>I29-H29</f>
         <v>9</v>
       </c>
-      <c r="K29" s="1">
-        <v>8.3000000000000004E-2</v>
+      <c r="K29" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
       <c r="L29" s="1">
-        <f>I29*K29</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M29" s="1">
+        <f>H29*L29</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N29" s="1">
+        <f>I29*L29</f>
         <v>0.83000000000000007</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I30" s="2">
+        <v>10</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L30" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M30" s="1">
+        <f>H30*L30</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N30" s="1">
+        <f>I30*L30</f>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G30" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H30" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I30" s="2">
-        <v>10</v>
-      </c>
-      <c r="J30" s="2">
+      <c r="G31" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I31" s="2">
+        <v>10</v>
+      </c>
+      <c r="J31" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="K30" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L30" s="1">
-        <f t="shared" si="3"/>
+      <c r="K31" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L31" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M31" s="1">
+        <f>H31*L31</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N31" s="1">
+        <f>I31*L31</f>
         <v>0.83000000000000007</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B31" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="2" t="s">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G31" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H31" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I31" s="2">
-        <v>10</v>
-      </c>
-      <c r="J31" s="2">
+      <c r="G32" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I32" s="2">
+        <v>10</v>
+      </c>
+      <c r="J32" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="K31" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L31" s="1">
-        <f t="shared" si="3"/>
+      <c r="K32" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L32" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M32" s="1">
+        <f>H32*L32</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N32" s="1">
+        <f>I32*L32</f>
         <v>0.83000000000000007</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I33" s="2">
+        <v>10</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L33" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M33" s="1">
+        <f>H33*L33</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N33" s="1">
+        <f>I33*L33</f>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H32" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I32" s="2">
-        <v>10</v>
-      </c>
-      <c r="J32" s="2">
+      <c r="B34" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I34" s="2">
+        <v>10</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="L34" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M34" s="1">
+        <f>H34*L34</f>
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="N34" s="1">
+        <f>I34*L34</f>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I35" s="2">
+        <v>10</v>
+      </c>
+      <c r="J35" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="K32" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L32" s="1">
-        <f t="shared" si="3"/>
+      <c r="K35" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L35" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M35" s="1">
+        <f>H35*L35</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N35" s="1">
+        <f>I35*L35</f>
         <v>0.83000000000000007</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H33" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I33" s="2">
-        <v>10</v>
-      </c>
-      <c r="J33" s="2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I36" s="2">
+        <v>10</v>
+      </c>
+      <c r="J36" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="K33" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L33" s="1">
-        <f t="shared" si="3"/>
+      <c r="K36" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L36" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M36" s="1">
+        <f>H36*L36</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N36" s="1">
+        <f>I36*L36</f>
         <v>0.83000000000000007</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H34" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I34" s="2">
-        <v>10</v>
-      </c>
-      <c r="J34" s="2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I37" s="2">
+        <v>10</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L37" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="M37" s="1">
+        <f>H37*L37</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N37" s="1">
+        <f>I37*L37</f>
+        <v>0.83000000000000007</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I38" s="2">
+        <v>10</v>
+      </c>
+      <c r="J38" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="K34" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L34" s="1">
-        <f t="shared" si="3"/>
-        <v>0.83000000000000007</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H35" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I35" s="2">
-        <v>10</v>
-      </c>
-      <c r="J35" s="2">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="K35" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L35" s="1">
-        <f t="shared" si="3"/>
-        <v>0.83000000000000007</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H36" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I36" s="2">
-        <v>10</v>
-      </c>
-      <c r="J36" s="2">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="K36" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L36" s="1">
-        <f t="shared" si="3"/>
-        <v>0.83000000000000007</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B37" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H37" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I37" s="2">
-        <v>10</v>
-      </c>
-      <c r="J37" s="2">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="K37" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L37" s="1">
-        <f t="shared" si="3"/>
-        <v>0.83000000000000007</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="K38" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="L38" s="1">
+        <v>1.2E-2</v>
+      </c>
+      <c r="M38" s="1">
+        <f>H38*L38</f>
+        <v>2.4E-2</v>
+      </c>
+      <c r="N38" s="1">
+        <f>I38*L38</f>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G38" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H38" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I38" s="2">
-        <v>10</v>
-      </c>
-      <c r="J38" s="2">
+      <c r="G39" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I39" s="2">
+        <v>10</v>
+      </c>
+      <c r="J39" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="K38" s="1">
-        <v>1.2E-2</v>
-      </c>
-      <c r="L38" s="1">
-        <f t="shared" si="3"/>
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B39" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="K39" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="L39" s="1">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="M39" s="1">
+        <f>H39*L39</f>
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="N39" s="1">
+        <f>I39*L39</f>
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B40" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F39" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="G39" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H39" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I39" s="2">
-        <v>10</v>
-      </c>
-      <c r="J39" s="2">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="K39" s="1">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="L39" s="1">
-        <f t="shared" si="3"/>
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B40" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="G40" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" si="1"/>
@@ -2705,36 +3026,44 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K40" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="L40" s="1">
         <v>4.6600000000000003E-2</v>
       </c>
-      <c r="L40" s="1">
-        <f t="shared" si="3"/>
+      <c r="M40" s="1">
+        <f>H40*L40</f>
+        <v>0.37280000000000002</v>
+      </c>
+      <c r="N40" s="1">
+        <f>I40*L40</f>
         <v>2.33</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B41" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G41" s="12" t="s">
         <v>90</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>93</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" si="1"/>
@@ -2747,37 +3076,45 @@
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K41" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="L41" s="1">
         <v>0.13059999999999999</v>
       </c>
-      <c r="L41" s="1">
-        <f t="shared" si="3"/>
+      <c r="M41" s="1">
+        <f>H41*L41</f>
+        <v>0.9141999999999999</v>
+      </c>
+      <c r="N41" s="1">
+        <f>I41*L41</f>
         <v>6.5299999999999994</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B42" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G42" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>182</v>
-      </c>
       <c r="H42" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2789,36 +3126,44 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K42" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L42" s="1">
         <v>0.51300000000000001</v>
       </c>
-      <c r="L42" s="1">
-        <f t="shared" si="3"/>
+      <c r="M42" s="1">
+        <f>H42*L42</f>
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="N42" s="1">
+        <f>I42*L42</f>
         <v>5.13</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B43" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" si="1"/>
@@ -2831,37 +3176,45 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="K43" s="1">
+      <c r="K43" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="L43" s="1">
         <v>0.55600000000000005</v>
       </c>
-      <c r="L43" s="1">
-        <f t="shared" si="3"/>
+      <c r="M43" s="1">
+        <f>H43*L43</f>
+        <v>1.6680000000000001</v>
+      </c>
+      <c r="N43" s="1">
+        <f>I43*L43</f>
         <v>5.5600000000000005</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B44" s="2">
         <f>1+LEN(A44)-LEN(SUBSTITUTE(A44,",",""))</f>
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E44" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G44" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G44" s="12" t="s">
-        <v>187</v>
-      </c>
       <c r="H44" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2873,36 +3226,44 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L44" s="1">
         <v>0.41899999999999998</v>
       </c>
-      <c r="L44" s="1">
-        <f t="shared" si="3"/>
+      <c r="M44" s="1">
+        <f>H44*L44</f>
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="N44" s="1">
+        <f>I44*L44</f>
         <v>4.1899999999999995</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B45" s="2">
         <f>1+LEN(A45)-LEN(SUBSTITUTE(A45,",",""))</f>
         <v>16</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" si="1"/>
@@ -2915,33 +3276,41 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="K45" s="1">
+      <c r="K45" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="L45" s="1">
         <v>0.41599999999999998</v>
       </c>
-      <c r="L45" s="1">
-        <f t="shared" si="3"/>
+      <c r="M45" s="1">
+        <f>H45*L45</f>
+        <v>6.6559999999999997</v>
+      </c>
+      <c r="N45" s="1">
+        <f>I45*L45</f>
         <v>20.8</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B46" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="2">
@@ -2955,36 +3324,44 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="K46" s="1">
+      <c r="K46" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="L46" s="1">
         <v>0.32700000000000001</v>
       </c>
-      <c r="L46" s="1">
-        <f t="shared" si="3"/>
+      <c r="M46" s="1">
+        <f>H46*L46</f>
+        <v>2.6160000000000001</v>
+      </c>
+      <c r="N46" s="1">
+        <f>I46*L46</f>
         <v>9.81</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B47" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" si="1"/>
@@ -2997,15 +3374,23 @@
         <f t="shared" si="2"/>
         <v>-5</v>
       </c>
-      <c r="K47" s="1">
+      <c r="K47" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L47" s="1">
         <v>5.56</v>
       </c>
-      <c r="L47" s="1">
-        <f t="shared" si="3"/>
+      <c r="M47" s="1">
+        <f>L47</f>
         <v>5.56</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N47" s="1">
+        <f>I47*L47</f>
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>4</v>
       </c>
@@ -3018,10 +3403,15 @@
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="16">
-        <f>SUM(L2:L47)</f>
-        <v>237.72000000000028</v>
+      <c r="K48" s="14"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10">
+        <f>SUM(M2:M47)</f>
+        <v>63.522999999999961</v>
+      </c>
+      <c r="N48" s="16">
+        <f>SUM(N2:N47)</f>
+        <v>172.27999999999994</v>
       </c>
     </row>
   </sheetData>
@@ -3030,7 +3420,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L47">
+  <conditionalFormatting sqref="N2:N47">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Created all of the custom footprints necessary.
Also updated the BOM to include the footprints used.
</commit_message>
<xml_diff>
--- a/KiCad/Power_Board/BOM.xlsx
+++ b/KiCad/Power_Board/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="221">
   <si>
     <t>REFDES</t>
   </si>
@@ -342,9 +342,6 @@
     <t>1N5261B-ND</t>
   </si>
   <si>
-    <t>THROUGH-HOLE</t>
-  </si>
-  <si>
     <t>541-1.00KLCT-ND</t>
   </si>
   <si>
@@ -618,9 +615,6 @@
     <t>GBC36SBSN-M89</t>
   </si>
   <si>
-    <t>CUT TO SIZE</t>
-  </si>
-  <si>
     <t>Board Total</t>
   </si>
   <si>
@@ -637,6 +631,54 @@
   </si>
   <si>
     <t>8 Channel 8bit DAC</t>
+  </si>
+  <si>
+    <t>SOT_323</t>
+  </si>
+  <si>
+    <t>SOT_223</t>
+  </si>
+  <si>
+    <t>DO-35</t>
+  </si>
+  <si>
+    <t>CUSTOM (NRS5030)</t>
+  </si>
+  <si>
+    <t>CUSTOM (QSOP_16)</t>
+  </si>
+  <si>
+    <t>CUSTOM (SOT_623)</t>
+  </si>
+  <si>
+    <t>CUSTOM (TPS63030)</t>
+  </si>
+  <si>
+    <t>CUSTOM (ADP5070)</t>
+  </si>
+  <si>
+    <t>CUSTOM (ADP7142)</t>
+  </si>
+  <si>
+    <t>CUSTOM (ADP7182)</t>
+  </si>
+  <si>
+    <t>CUSTOM (ADP3335)</t>
+  </si>
+  <si>
+    <t>CUSTOM (DFLS240)</t>
+  </si>
+  <si>
+    <t>CUSTOM (1N4148)</t>
+  </si>
+  <si>
+    <t>CUSTOM (NS12555)</t>
+  </si>
+  <si>
+    <t>CUSTOM (TEST_CLIP)</t>
+  </si>
+  <si>
+    <t>CUSTOM (SMD_JUMPER)</t>
   </si>
 </sst>
 </file>
@@ -735,17 +777,7 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1055,9 +1087,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N41" sqref="N41"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1099,7 @@
     <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="14.42578125" customWidth="1"/>
@@ -1108,16 +1140,16 @@
         <v>47</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1140,7 +1172,9 @@
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="12" t="s">
+        <v>211</v>
+      </c>
       <c r="H2" s="2">
         <f t="shared" ref="H2:H47" si="1">B2</f>
         <v>4</v>
@@ -1160,11 +1194,11 @@
         <v>2.25</v>
       </c>
       <c r="M2" s="1">
-        <f>H2*L2</f>
+        <f t="shared" ref="M2:M46" si="3">H2*L2</f>
         <v>9</v>
       </c>
       <c r="N2" s="1">
-        <f>I2*L2</f>
+        <f t="shared" ref="N2:N47" si="4">I2*L2</f>
         <v>22.5</v>
       </c>
     </row>
@@ -1188,7 +1222,9 @@
       <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="12"/>
+      <c r="G3" s="12" t="s">
+        <v>212</v>
+      </c>
       <c r="H3" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1201,18 +1237,18 @@
         <v>1</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" ref="K3:K47" si="3">FLOOR(I3/H3,1)</f>
+        <f t="shared" ref="K3:K47" si="5">FLOOR(I3/H3,1)</f>
         <v>2</v>
       </c>
       <c r="L3" s="1">
         <v>5.99</v>
       </c>
       <c r="M3" s="1">
-        <f>H3*L3</f>
+        <f t="shared" si="3"/>
         <v>5.99</v>
       </c>
       <c r="N3" s="1">
-        <f>I3*L3</f>
+        <f t="shared" si="4"/>
         <v>11.98</v>
       </c>
     </row>
@@ -1236,7 +1272,9 @@
       <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="12" t="s">
+        <v>213</v>
+      </c>
       <c r="H4" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1249,18 +1287,18 @@
         <v>1</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L4" s="1">
         <v>3.06</v>
       </c>
       <c r="M4" s="1">
-        <f>H4*L4</f>
+        <f t="shared" si="3"/>
         <v>3.06</v>
       </c>
       <c r="N4" s="1">
-        <f>I4*L4</f>
+        <f t="shared" si="4"/>
         <v>6.12</v>
       </c>
     </row>
@@ -1284,7 +1322,9 @@
       <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>214</v>
+      </c>
       <c r="H5" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1297,18 +1337,18 @@
         <v>1</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L5" s="1">
         <v>3.65</v>
       </c>
       <c r="M5" s="1">
-        <f>H5*L5</f>
+        <f t="shared" si="3"/>
         <v>3.65</v>
       </c>
       <c r="N5" s="1">
-        <f>I5*L5</f>
+        <f t="shared" si="4"/>
         <v>7.3</v>
       </c>
     </row>
@@ -1332,7 +1372,9 @@
       <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="12"/>
+      <c r="G6" s="12" t="s">
+        <v>215</v>
+      </c>
       <c r="H6" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1345,18 +1387,18 @@
         <v>1</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L6" s="1">
         <v>2.76</v>
       </c>
       <c r="M6" s="1">
-        <f>H6*L6</f>
+        <f t="shared" si="3"/>
         <v>2.76</v>
       </c>
       <c r="N6" s="1">
-        <f>I6*L6</f>
+        <f t="shared" si="4"/>
         <v>5.52</v>
       </c>
     </row>
@@ -1380,7 +1422,9 @@
       <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="12" t="s">
+        <v>210</v>
+      </c>
       <c r="H7" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1393,18 +1437,18 @@
         <v>1</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L7" s="1">
         <v>3.84</v>
       </c>
       <c r="M7" s="1">
-        <f>H7*L7</f>
+        <f t="shared" si="3"/>
         <v>3.84</v>
       </c>
       <c r="N7" s="1">
-        <f>I7*L7</f>
+        <f t="shared" si="4"/>
         <v>7.68</v>
       </c>
     </row>
@@ -1420,15 +1464,17 @@
         <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="12" t="s">
+        <v>209</v>
+      </c>
       <c r="H8" s="2">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -1441,18 +1487,18 @@
         <v>2</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L8" s="1">
         <v>2.82</v>
       </c>
       <c r="M8" s="1">
-        <f>H8*L8</f>
+        <f t="shared" si="3"/>
         <v>5.64</v>
       </c>
       <c r="N8" s="1">
-        <f>I8*L8</f>
+        <f t="shared" si="4"/>
         <v>11.28</v>
       </c>
     </row>
@@ -1476,7 +1522,9 @@
       <c r="F9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="12"/>
+      <c r="G9" s="12" t="s">
+        <v>205</v>
+      </c>
       <c r="H9" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1489,18 +1537,18 @@
         <v>1</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L9" s="1">
         <v>2.27</v>
       </c>
       <c r="M9" s="1">
-        <f>H9*L9</f>
+        <f t="shared" si="3"/>
         <v>2.27</v>
       </c>
       <c r="N9" s="1">
-        <f>I9*L9</f>
+        <f t="shared" si="4"/>
         <v>4.54</v>
       </c>
     </row>
@@ -1524,7 +1572,9 @@
       <c r="F10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="G10" s="12" t="s">
+        <v>206</v>
+      </c>
       <c r="H10" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1537,18 +1587,18 @@
         <v>2</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L10" s="1">
         <v>0.93</v>
       </c>
       <c r="M10" s="1">
-        <f>H10*L10</f>
+        <f t="shared" si="3"/>
         <v>0.93</v>
       </c>
       <c r="N10" s="1">
-        <f>I10*L10</f>
+        <f t="shared" si="4"/>
         <v>2.79</v>
       </c>
     </row>
@@ -1572,7 +1622,9 @@
       <c r="F11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="G11" s="12" t="s">
+        <v>216</v>
+      </c>
       <c r="H11" s="2">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -1585,18 +1637,18 @@
         <v>3</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L11" s="1">
         <v>0.46</v>
       </c>
       <c r="M11" s="1">
-        <f>H11*L11</f>
+        <f t="shared" si="3"/>
         <v>0.92</v>
       </c>
       <c r="N11" s="1">
-        <f>I11*L11</f>
+        <f t="shared" si="4"/>
         <v>2.3000000000000003</v>
       </c>
     </row>
@@ -1620,7 +1672,9 @@
       <c r="F12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="12"/>
+      <c r="G12" s="12" t="s">
+        <v>217</v>
+      </c>
       <c r="H12" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1633,18 +1687,18 @@
         <v>9</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L12" s="1">
         <v>0.14599999999999999</v>
       </c>
       <c r="M12" s="1">
-        <f>H12*L12</f>
+        <f t="shared" si="3"/>
         <v>0.14599999999999999</v>
       </c>
       <c r="N12" s="1">
-        <f>I12*L12</f>
+        <f t="shared" si="4"/>
         <v>1.46</v>
       </c>
     </row>
@@ -1669,7 +1723,7 @@
         <v>81</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>108</v>
+        <v>207</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="1"/>
@@ -1683,18 +1737,18 @@
         <v>9</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L13" s="1">
         <v>0.11700000000000001</v>
       </c>
       <c r="M13" s="1">
-        <f>H13*L13</f>
+        <f t="shared" si="3"/>
         <v>0.11700000000000001</v>
       </c>
       <c r="N13" s="1">
-        <f>I13*L13</f>
+        <f t="shared" si="4"/>
         <v>1.1700000000000002</v>
       </c>
     </row>
@@ -1718,7 +1772,9 @@
       <c r="F14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="12"/>
+      <c r="G14" s="12" t="s">
+        <v>208</v>
+      </c>
       <c r="H14" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1731,18 +1787,18 @@
         <v>5</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L14" s="1">
         <v>0.41</v>
       </c>
       <c r="M14" s="1">
-        <f>H14*L14</f>
+        <f t="shared" si="3"/>
         <v>2.0499999999999998</v>
       </c>
       <c r="N14" s="1">
-        <f>I14*L14</f>
+        <f t="shared" si="4"/>
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -1766,7 +1822,9 @@
       <c r="F15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="12"/>
+      <c r="G15" s="12" t="s">
+        <v>208</v>
+      </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1779,18 +1837,18 @@
         <v>2</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L15" s="1">
         <v>0.46</v>
       </c>
       <c r="M15" s="1">
-        <f>H15*L15</f>
+        <f t="shared" si="3"/>
         <v>0.46</v>
       </c>
       <c r="N15" s="1">
-        <f>I15*L15</f>
+        <f t="shared" si="4"/>
         <v>1.3800000000000001</v>
       </c>
     </row>
@@ -1814,7 +1872,9 @@
       <c r="F16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="12" t="s">
+        <v>218</v>
+      </c>
       <c r="H16" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1827,18 +1887,18 @@
         <v>1</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L16" s="1">
         <v>1.41</v>
       </c>
       <c r="M16" s="1">
-        <f>H16*L16</f>
+        <f t="shared" si="3"/>
         <v>1.41</v>
       </c>
       <c r="N16" s="1">
-        <f>I16*L16</f>
+        <f t="shared" si="4"/>
         <v>2.82</v>
       </c>
     </row>
@@ -1854,16 +1914,16 @@
         <v>34</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="1"/>
@@ -1877,18 +1937,18 @@
         <v>42</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L17" s="1">
         <v>0.04</v>
       </c>
       <c r="M17" s="1">
-        <f>H17*L17</f>
+        <f t="shared" si="3"/>
         <v>0.32</v>
       </c>
       <c r="N17" s="1">
-        <f>I17*L17</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -1904,17 +1964,17 @@
         <v>34</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>111</v>
-      </c>
       <c r="H18" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1927,18 +1987,18 @@
         <v>9</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L18" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M18" s="1">
-        <f>H18*L18</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N18" s="1">
-        <f>I18*L18</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -1954,16 +2014,16 @@
         <v>34</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="1"/>
@@ -1977,18 +2037,18 @@
         <v>9</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L19" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M19" s="1">
-        <f>H19*L19</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N19" s="1">
-        <f>I19*L19</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2004,16 +2064,16 @@
         <v>34</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="G20" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="1"/>
@@ -2027,18 +2087,18 @@
         <v>7</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L20" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M20" s="1">
-        <f>H20*L20</f>
+        <f t="shared" si="3"/>
         <v>0.249</v>
       </c>
       <c r="N20" s="1">
-        <f>I20*L20</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2054,16 +2114,16 @@
         <v>34</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="G21" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="1"/>
@@ -2077,43 +2137,43 @@
         <v>9</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L21" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M21" s="1">
-        <f>H21*L21</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N21" s="1">
-        <f>I21*L21</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B22" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="G22" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="1"/>
@@ -2127,18 +2187,18 @@
         <v>8</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L22" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M22" s="1">
-        <f>H22*L22</f>
+        <f t="shared" si="3"/>
         <v>0.16600000000000001</v>
       </c>
       <c r="N22" s="1">
-        <f>I22*L22</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2154,16 +2214,16 @@
         <v>34</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="G23" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" si="1"/>
@@ -2177,18 +2237,18 @@
         <v>9</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L23" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M23" s="1">
-        <f>H23*L23</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N23" s="1">
-        <f>I23*L23</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2204,16 +2264,16 @@
         <v>34</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="G24" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" si="1"/>
@@ -2227,18 +2287,18 @@
         <v>9</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L24" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M24" s="1">
-        <f>H24*L24</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N24" s="1">
-        <f>I24*L24</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2254,16 +2314,16 @@
         <v>34</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="G25" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="1"/>
@@ -2277,18 +2337,18 @@
         <v>9</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L25" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M25" s="1">
-        <f>H25*L25</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N25" s="1">
-        <f>I25*L25</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2304,16 +2364,16 @@
         <v>34</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="G26" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="1"/>
@@ -2327,18 +2387,18 @@
         <v>9</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L26" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M26" s="1">
-        <f>H26*L26</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N26" s="1">
-        <f>I26*L26</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2354,16 +2414,16 @@
         <v>34</v>
       </c>
       <c r="D27" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" si="1"/>
@@ -2377,18 +2437,18 @@
         <v>9</v>
       </c>
       <c r="K27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L27" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M27" s="1">
-        <f>H27*L27</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N27" s="1">
-        <f>I27*L27</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2404,16 +2464,16 @@
         <v>34</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="G28" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H28" s="2">
         <f>B28</f>
@@ -2427,18 +2487,18 @@
         <v>8</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L28" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M28" s="1">
-        <f>H28*L28</f>
+        <f t="shared" si="3"/>
         <v>0.16600000000000001</v>
       </c>
       <c r="N28" s="1">
-        <f>I28*L28</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2454,16 +2514,16 @@
         <v>34</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="G29" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H29" s="2">
         <f>B29</f>
@@ -2477,18 +2537,18 @@
         <v>9</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L29" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M29" s="1">
-        <f>H29*L29</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N29" s="1">
-        <f>I29*L29</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2504,16 +2564,16 @@
         <v>34</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="G30" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="1"/>
@@ -2527,18 +2587,18 @@
         <v>9</v>
       </c>
       <c r="K30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L30" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M30" s="1">
-        <f>H30*L30</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N30" s="1">
-        <f>I30*L30</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2554,16 +2614,16 @@
         <v>34</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="G31" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" si="1"/>
@@ -2577,18 +2637,18 @@
         <v>9</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L31" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M31" s="1">
-        <f>H31*L31</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N31" s="1">
-        <f>I31*L31</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2604,16 +2664,16 @@
         <v>34</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="G32" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" si="1"/>
@@ -2627,18 +2687,18 @@
         <v>9</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L32" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M32" s="1">
-        <f>H32*L32</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N32" s="1">
-        <f>I32*L32</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2654,16 +2714,16 @@
         <v>34</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="G33" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" si="1"/>
@@ -2677,18 +2737,18 @@
         <v>9</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L33" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M33" s="1">
-        <f>H33*L33</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N33" s="1">
-        <f>I33*L33</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2704,16 +2764,16 @@
         <v>34</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="G34" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" si="1"/>
@@ -2727,18 +2787,18 @@
         <v>8</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L34" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M34" s="1">
-        <f>H34*L34</f>
+        <f t="shared" si="3"/>
         <v>0.16600000000000001</v>
       </c>
       <c r="N34" s="1">
-        <f>I34*L34</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2754,16 +2814,16 @@
         <v>34</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="G35" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" si="1"/>
@@ -2777,18 +2837,18 @@
         <v>9</v>
       </c>
       <c r="K35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L35" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M35" s="1">
-        <f>H35*L35</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N35" s="1">
-        <f>I35*L35</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2804,16 +2864,16 @@
         <v>34</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="G36" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H36" s="2">
         <f t="shared" si="1"/>
@@ -2827,18 +2887,18 @@
         <v>9</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L36" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M36" s="1">
-        <f>H36*L36</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N36" s="1">
-        <f>I36*L36</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2854,13 +2914,13 @@
         <v>34</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="G37" s="12" t="s">
         <v>90</v>
@@ -2877,18 +2937,18 @@
         <v>9</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L37" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M37" s="1">
-        <f>H37*L37</f>
+        <f t="shared" si="3"/>
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="N37" s="1">
-        <f>I37*L37</f>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
     </row>
@@ -2904,16 +2964,16 @@
         <v>34</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="G38" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H38" s="2">
         <f t="shared" si="1"/>
@@ -2927,18 +2987,18 @@
         <v>8</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L38" s="1">
         <v>1.2E-2</v>
       </c>
       <c r="M38" s="1">
-        <f>H38*L38</f>
+        <f t="shared" si="3"/>
         <v>2.4E-2</v>
       </c>
       <c r="N38" s="1">
-        <f>I38*L38</f>
+        <f t="shared" si="4"/>
         <v>0.12</v>
       </c>
     </row>
@@ -2954,16 +3014,16 @@
         <v>34</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="G39" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="1"/>
@@ -2977,24 +3037,24 @@
         <v>8</v>
       </c>
       <c r="K39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L39" s="1">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="M39" s="1">
-        <f>H39*L39</f>
+        <f t="shared" si="3"/>
         <v>0.14199999999999999</v>
       </c>
       <c r="N39" s="1">
-        <f>I39*L39</f>
+        <f t="shared" si="4"/>
         <v>0.71</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B40" s="2">
         <f t="shared" si="0"/>
@@ -3004,13 +3064,13 @@
         <v>34</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>90</v>
@@ -3027,18 +3087,18 @@
         <v>42</v>
       </c>
       <c r="K40" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L40" s="1">
         <v>4.6600000000000003E-2</v>
       </c>
       <c r="M40" s="1">
-        <f>H40*L40</f>
+        <f t="shared" si="3"/>
         <v>0.37280000000000002</v>
       </c>
       <c r="N40" s="1">
-        <f>I40*L40</f>
+        <f t="shared" si="4"/>
         <v>2.33</v>
       </c>
     </row>
@@ -3060,7 +3120,7 @@
         <v>88</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>90</v>
@@ -3077,18 +3137,18 @@
         <v>43</v>
       </c>
       <c r="K41" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="L41" s="1">
         <v>0.13059999999999999</v>
       </c>
       <c r="M41" s="1">
-        <f>H41*L41</f>
+        <f t="shared" si="3"/>
         <v>0.9141999999999999</v>
       </c>
       <c r="N41" s="1">
-        <f>I41*L41</f>
+        <f t="shared" si="4"/>
         <v>6.5299999999999994</v>
       </c>
     </row>
@@ -3104,17 +3164,17 @@
         <v>34</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="G42" s="12" t="s">
-        <v>179</v>
-      </c>
       <c r="H42" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3127,18 +3187,18 @@
         <v>9</v>
       </c>
       <c r="K42" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L42" s="1">
         <v>0.51300000000000001</v>
       </c>
       <c r="M42" s="1">
-        <f>H42*L42</f>
+        <f t="shared" si="3"/>
         <v>0.51300000000000001</v>
       </c>
       <c r="N42" s="1">
-        <f>I42*L42</f>
+        <f t="shared" si="4"/>
         <v>5.13</v>
       </c>
     </row>
@@ -3154,16 +3214,16 @@
         <v>34</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="G43" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" si="1"/>
@@ -3177,18 +3237,18 @@
         <v>7</v>
       </c>
       <c r="K43" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L43" s="1">
         <v>0.55600000000000005</v>
       </c>
       <c r="M43" s="1">
-        <f>H43*L43</f>
+        <f t="shared" si="3"/>
         <v>1.6680000000000001</v>
       </c>
       <c r="N43" s="1">
-        <f>I43*L43</f>
+        <f t="shared" si="4"/>
         <v>5.5600000000000005</v>
       </c>
     </row>
@@ -3204,16 +3264,16 @@
         <v>34</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="G44" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" si="1"/>
@@ -3227,18 +3287,18 @@
         <v>9</v>
       </c>
       <c r="K44" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L44" s="1">
         <v>0.41899999999999998</v>
       </c>
       <c r="M44" s="1">
-        <f>H44*L44</f>
+        <f t="shared" si="3"/>
         <v>0.41899999999999998</v>
       </c>
       <c r="N44" s="1">
-        <f>I44*L44</f>
+        <f t="shared" si="4"/>
         <v>4.1899999999999995</v>
       </c>
     </row>
@@ -3260,7 +3320,7 @@
         <v>93</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>91</v>
@@ -3277,18 +3337,18 @@
         <v>34</v>
       </c>
       <c r="K45" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L45" s="1">
         <v>0.41599999999999998</v>
       </c>
       <c r="M45" s="1">
-        <f>H45*L45</f>
+        <f t="shared" si="3"/>
         <v>6.6559999999999997</v>
       </c>
       <c r="N45" s="1">
-        <f>I45*L45</f>
+        <f t="shared" si="4"/>
         <v>20.8</v>
       </c>
     </row>
@@ -3304,15 +3364,17 @@
         <v>34</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G46" s="12"/>
+      <c r="G46" s="12" t="s">
+        <v>219</v>
+      </c>
       <c r="H46" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -3325,18 +3387,18 @@
         <v>22</v>
       </c>
       <c r="K46" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L46" s="1">
         <v>0.32700000000000001</v>
       </c>
       <c r="M46" s="1">
-        <f>H46*L46</f>
+        <f t="shared" si="3"/>
         <v>2.6160000000000001</v>
       </c>
       <c r="N46" s="1">
-        <f>I46*L46</f>
+        <f t="shared" si="4"/>
         <v>9.81</v>
       </c>
     </row>
@@ -3352,16 +3414,16 @@
         <v>34</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>199</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>42</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" si="1"/>
@@ -3375,7 +3437,7 @@
         <v>-5</v>
       </c>
       <c r="K47" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L47" s="1">
@@ -3386,7 +3448,7 @@
         <v>5.56</v>
       </c>
       <c r="N47" s="1">
-        <f>I47*L47</f>
+        <f t="shared" si="4"/>
         <v>5.56</v>
       </c>
     </row>
@@ -3416,7 +3478,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Linked footprints to schematic.
Also cleaned up some footprint errors:
Changed IC footprint names to be invisible on the silkscreen layer.
Fixed test points that were lacking pin numbers causing netlist
failures.
</commit_message>
<xml_diff>
--- a/KiCad/Power_Board/BOM.xlsx
+++ b/KiCad/Power_Board/BOM.xlsx
@@ -1085,11 +1085,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3495,7 +3498,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="44" orientation="landscape" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>